<commit_message>
update calcs in hosp
</commit_message>
<xml_diff>
--- a/ped hosp.xlsx
+++ b/ped hosp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timwiemken/Library/Mobile Documents/com~apple~CloudDocs/Work/Pfizer/COVID pediatric case count/count github/covid-agegroups/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0F14267A-AE53-BD41-93F7-A51981E91CF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC901FAF-FBA1-1842-8FB3-D36E6642B5B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15000" yWindow="500" windowWidth="13800" windowHeight="17500" xr2:uid="{916C03D1-2999-1643-8854-B7147CC86D48}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>report_date</t>
   </si>
@@ -43,6 +43,15 @@
   </si>
   <si>
     <t xml:space="preserve">Pop 2020 </t>
+  </si>
+  <si>
+    <t>Aug/sep</t>
+  </si>
+  <si>
+    <t>In last 2 months</t>
+  </si>
+  <si>
+    <t>Aug/Aug</t>
   </si>
 </sst>
 </file>
@@ -403,10 +412,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{389612D9-AD97-814B-96F2-ACB2873AC0FE}">
-  <dimension ref="A1:E431"/>
+  <dimension ref="A1:F438"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A315" workbookViewId="0">
-      <selection activeCell="C432" sqref="C432"/>
+    <sheetView tabSelected="1" topLeftCell="A418" workbookViewId="0">
+      <selection activeCell="G436" sqref="G436"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5398,7 +5407,7 @@
         <v>327.69950850000004</v>
       </c>
     </row>
-    <row r="417" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="417" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A417" s="1">
         <v>44458</v>
       </c>
@@ -5410,7 +5419,7 @@
         <v>320.41729720000001</v>
       </c>
     </row>
-    <row r="418" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="418" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A418" s="1">
         <v>44459</v>
       </c>
@@ -5422,7 +5431,7 @@
         <v>313.13508589999998</v>
       </c>
     </row>
-    <row r="419" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="419" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A419" s="1">
         <v>44460</v>
       </c>
@@ -5434,7 +5443,7 @@
         <v>298.57066329999998</v>
       </c>
     </row>
-    <row r="420" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="420" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A420" s="1">
         <v>44461</v>
       </c>
@@ -5446,7 +5455,7 @@
         <v>284.00624069999998</v>
       </c>
     </row>
-    <row r="421" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="421" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A421" s="1">
         <v>44462</v>
       </c>
@@ -5458,7 +5467,7 @@
         <v>276.72402940000001</v>
       </c>
     </row>
-    <row r="422" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="422" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A422" s="1">
         <v>44463</v>
       </c>
@@ -5470,7 +5479,7 @@
         <v>276.72402940000001</v>
       </c>
     </row>
-    <row r="423" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="423" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A423" s="1">
         <v>44464</v>
       </c>
@@ -5482,7 +5491,7 @@
         <v>269.44181809999998</v>
       </c>
     </row>
-    <row r="424" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="424" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A424" s="1">
         <v>44465</v>
       </c>
@@ -5494,7 +5503,7 @@
         <v>262.15960680000001</v>
       </c>
     </row>
-    <row r="425" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="425" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A425" s="1">
         <v>44466</v>
       </c>
@@ -5506,7 +5515,7 @@
         <v>254.87739549999998</v>
       </c>
     </row>
-    <row r="426" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="426" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A426" s="1">
         <v>44467</v>
       </c>
@@ -5518,7 +5527,7 @@
         <v>254.87739549999998</v>
       </c>
     </row>
-    <row r="427" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="427" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A427" s="1">
         <v>44468</v>
       </c>
@@ -5530,10 +5539,35 @@
         <v>247.59518420000001</v>
       </c>
     </row>
-    <row r="431" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="431" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C431" s="2">
         <f>SUM(C3:C427)</f>
         <v>61556.53211890033</v>
+      </c>
+      <c r="E431" s="2">
+        <f>SUM(C3:C367)</f>
+        <v>43678.703377400278</v>
+      </c>
+      <c r="F431" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="432" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E432" s="2">
+        <f>SUM(C368:C427)</f>
+        <v>17877.828741500009</v>
+      </c>
+      <c r="F432" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="438" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D438">
+        <f>E432/C431*100</f>
+        <v>29.042943333727528</v>
+      </c>
+      <c r="E438" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating app to add hospitalizations
</commit_message>
<xml_diff>
--- a/ped hosp.xlsx
+++ b/ped hosp.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pfizer-my.sharepoint.com/personal/wiemkt_pfizer_com/Documents/Documents/Research/covid-agegroups/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{EC901FAF-FBA1-1842-8FB3-D36E6642B5B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{FA4E9921-1B01-45B7-AD8E-F7D730DAA080}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{EC901FAF-FBA1-1842-8FB3-D36E6642B5B7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{163AE09C-C295-4E1B-81E6-0AFFD7E89E9F}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{916C03D1-2999-1643-8854-B7147CC86D48}"/>
+    <workbookView xWindow="2200" yWindow="2200" windowWidth="14400" windowHeight="7360" xr2:uid="{916C03D1-2999-1643-8854-B7147CC86D48}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -391,33 +391,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{389612D9-AD97-814B-96F2-ACB2873AC0FE}">
-  <dimension ref="A2:B427"/>
+  <dimension ref="A1:B426"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A420" workbookViewId="0">
-      <selection activeCell="E429" sqref="E429"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
+      <c r="A2" s="1">
+        <v>44044</v>
+      </c>
+      <c r="B2">
+        <v>0.14000000000000001</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
-        <v>44044</v>
+        <v>44045</v>
       </c>
       <c r="B3">
-        <v>0.14000000000000001</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
-        <v>44045</v>
+        <v>44046</v>
       </c>
       <c r="B4">
         <v>0.13</v>
@@ -425,7 +433,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
-        <v>44046</v>
+        <v>44047</v>
       </c>
       <c r="B5">
         <v>0.13</v>
@@ -433,7 +441,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
-        <v>44047</v>
+        <v>44048</v>
       </c>
       <c r="B6">
         <v>0.13</v>
@@ -441,23 +449,23 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
-        <v>44048</v>
+        <v>44049</v>
       </c>
       <c r="B7">
-        <v>0.13</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
-        <v>44049</v>
+        <v>44050</v>
       </c>
       <c r="B8">
-        <v>0.12</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
-        <v>44050</v>
+        <v>44051</v>
       </c>
       <c r="B9">
         <v>0.13</v>
@@ -465,15 +473,15 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
-        <v>44051</v>
+        <v>44052</v>
       </c>
       <c r="B10">
-        <v>0.13</v>
+        <v>0.14000000000000001</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
-        <v>44052</v>
+        <v>44053</v>
       </c>
       <c r="B11">
         <v>0.14000000000000001</v>
@@ -481,15 +489,15 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
-        <v>44053</v>
+        <v>44054</v>
       </c>
       <c r="B12">
-        <v>0.14000000000000001</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
-        <v>44054</v>
+        <v>44055</v>
       </c>
       <c r="B13">
         <v>0.15</v>
@@ -497,7 +505,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
-        <v>44055</v>
+        <v>44056</v>
       </c>
       <c r="B14">
         <v>0.15</v>
@@ -505,7 +513,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
-        <v>44056</v>
+        <v>44057</v>
       </c>
       <c r="B15">
         <v>0.15</v>
@@ -513,7 +521,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
-        <v>44057</v>
+        <v>44058</v>
       </c>
       <c r="B16">
         <v>0.15</v>
@@ -521,39 +529,39 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
-        <v>44058</v>
+        <v>44059</v>
       </c>
       <c r="B17">
-        <v>0.15</v>
+        <v>0.14000000000000001</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
-        <v>44059</v>
+        <v>44060</v>
       </c>
       <c r="B18">
-        <v>0.14000000000000001</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
-        <v>44060</v>
+        <v>44061</v>
       </c>
       <c r="B19">
-        <v>0.13</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
-        <v>44061</v>
+        <v>44062</v>
       </c>
       <c r="B20">
-        <v>0.12</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
-        <v>44062</v>
+        <v>44063</v>
       </c>
       <c r="B21">
         <v>0.11</v>
@@ -561,15 +569,15 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
-        <v>44063</v>
+        <v>44064</v>
       </c>
       <c r="B22">
-        <v>0.11</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
-        <v>44064</v>
+        <v>44065</v>
       </c>
       <c r="B23">
         <v>0.1</v>
@@ -577,15 +585,15 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
-        <v>44065</v>
+        <v>44066</v>
       </c>
       <c r="B24">
-        <v>0.1</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
-        <v>44066</v>
+        <v>44067</v>
       </c>
       <c r="B25">
         <v>0.11</v>
@@ -593,15 +601,15 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
-        <v>44067</v>
+        <v>44068</v>
       </c>
       <c r="B26">
-        <v>0.11</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
-        <v>44068</v>
+        <v>44069</v>
       </c>
       <c r="B27">
         <v>0.1</v>
@@ -609,15 +617,15 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
-        <v>44069</v>
+        <v>44070</v>
       </c>
       <c r="B28">
-        <v>0.1</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
-        <v>44070</v>
+        <v>44071</v>
       </c>
       <c r="B29">
         <v>0.11</v>
@@ -625,7 +633,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
-        <v>44071</v>
+        <v>44072</v>
       </c>
       <c r="B30">
         <v>0.11</v>
@@ -633,7 +641,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
-        <v>44072</v>
+        <v>44073</v>
       </c>
       <c r="B31">
         <v>0.11</v>
@@ -641,7 +649,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
-        <v>44073</v>
+        <v>44074</v>
       </c>
       <c r="B32">
         <v>0.11</v>
@@ -649,23 +657,23 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
-        <v>44074</v>
+        <v>44075</v>
       </c>
       <c r="B33">
-        <v>0.11</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
-        <v>44075</v>
+        <v>44076</v>
       </c>
       <c r="B34">
-        <v>0.12</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" s="1">
-        <v>44076</v>
+        <v>44077</v>
       </c>
       <c r="B35">
         <v>0.11</v>
@@ -673,15 +681,15 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" s="1">
-        <v>44077</v>
+        <v>44078</v>
       </c>
       <c r="B36">
-        <v>0.11</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" s="1">
-        <v>44078</v>
+        <v>44079</v>
       </c>
       <c r="B37">
         <v>0.12</v>
@@ -689,7 +697,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" s="1">
-        <v>44079</v>
+        <v>44080</v>
       </c>
       <c r="B38">
         <v>0.12</v>
@@ -697,15 +705,15 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" s="1">
-        <v>44080</v>
+        <v>44081</v>
       </c>
       <c r="B39">
-        <v>0.12</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" s="1">
-        <v>44081</v>
+        <v>44082</v>
       </c>
       <c r="B40">
         <v>0.11</v>
@@ -713,7 +721,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" s="1">
-        <v>44082</v>
+        <v>44083</v>
       </c>
       <c r="B41">
         <v>0.11</v>
@@ -721,7 +729,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" s="1">
-        <v>44083</v>
+        <v>44084</v>
       </c>
       <c r="B42">
         <v>0.11</v>
@@ -729,23 +737,23 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" s="1">
-        <v>44084</v>
+        <v>44085</v>
       </c>
       <c r="B43">
-        <v>0.11</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" s="1">
-        <v>44085</v>
+        <v>44086</v>
       </c>
       <c r="B44">
-        <v>0.1</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" s="1">
-        <v>44086</v>
+        <v>44087</v>
       </c>
       <c r="B45">
         <v>0.09</v>
@@ -753,7 +761,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" s="1">
-        <v>44087</v>
+        <v>44088</v>
       </c>
       <c r="B46">
         <v>0.09</v>
@@ -761,15 +769,15 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" s="1">
-        <v>44088</v>
+        <v>44089</v>
       </c>
       <c r="B47">
-        <v>0.09</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" s="1">
-        <v>44089</v>
+        <v>44090</v>
       </c>
       <c r="B48">
         <v>0.1</v>
@@ -777,7 +785,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" s="1">
-        <v>44090</v>
+        <v>44091</v>
       </c>
       <c r="B49">
         <v>0.1</v>
@@ -785,7 +793,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" s="1">
-        <v>44091</v>
+        <v>44092</v>
       </c>
       <c r="B50">
         <v>0.1</v>
@@ -793,7 +801,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" s="1">
-        <v>44092</v>
+        <v>44093</v>
       </c>
       <c r="B51">
         <v>0.1</v>
@@ -801,7 +809,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" s="1">
-        <v>44093</v>
+        <v>44094</v>
       </c>
       <c r="B52">
         <v>0.1</v>
@@ -809,7 +817,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" s="1">
-        <v>44094</v>
+        <v>44095</v>
       </c>
       <c r="B53">
         <v>0.1</v>
@@ -817,7 +825,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" s="1">
-        <v>44095</v>
+        <v>44096</v>
       </c>
       <c r="B54">
         <v>0.1</v>
@@ -825,7 +833,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" s="1">
-        <v>44096</v>
+        <v>44097</v>
       </c>
       <c r="B55">
         <v>0.1</v>
@@ -833,7 +841,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" s="1">
-        <v>44097</v>
+        <v>44098</v>
       </c>
       <c r="B56">
         <v>0.1</v>
@@ -841,7 +849,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" s="1">
-        <v>44098</v>
+        <v>44099</v>
       </c>
       <c r="B57">
         <v>0.1</v>
@@ -849,15 +857,15 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" s="1">
-        <v>44099</v>
+        <v>44100</v>
       </c>
       <c r="B58">
-        <v>0.1</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" s="1">
-        <v>44100</v>
+        <v>44101</v>
       </c>
       <c r="B59">
         <v>0.11</v>
@@ -865,7 +873,7 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" s="1">
-        <v>44101</v>
+        <v>44102</v>
       </c>
       <c r="B60">
         <v>0.11</v>
@@ -873,15 +881,15 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" s="1">
-        <v>44102</v>
+        <v>44103</v>
       </c>
       <c r="B61">
-        <v>0.11</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" s="1">
-        <v>44103</v>
+        <v>44104</v>
       </c>
       <c r="B62">
         <v>0.1</v>
@@ -889,7 +897,7 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" s="1">
-        <v>44104</v>
+        <v>44105</v>
       </c>
       <c r="B63">
         <v>0.1</v>
@@ -897,15 +905,15 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" s="1">
-        <v>44105</v>
+        <v>44106</v>
       </c>
       <c r="B64">
-        <v>0.1</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" s="1">
-        <v>44106</v>
+        <v>44107</v>
       </c>
       <c r="B65">
         <v>0.11</v>
@@ -913,7 +921,7 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" s="1">
-        <v>44107</v>
+        <v>44108</v>
       </c>
       <c r="B66">
         <v>0.11</v>
@@ -921,7 +929,7 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" s="1">
-        <v>44108</v>
+        <v>44109</v>
       </c>
       <c r="B67">
         <v>0.11</v>
@@ -929,15 +937,15 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" s="1">
-        <v>44109</v>
+        <v>44110</v>
       </c>
       <c r="B68">
-        <v>0.11</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" s="1">
-        <v>44110</v>
+        <v>44111</v>
       </c>
       <c r="B69">
         <v>0.12</v>
@@ -945,15 +953,15 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" s="1">
-        <v>44111</v>
+        <v>44112</v>
       </c>
       <c r="B70">
-        <v>0.12</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71" s="1">
-        <v>44112</v>
+        <v>44113</v>
       </c>
       <c r="B71">
         <v>0.13</v>
@@ -961,7 +969,7 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A72" s="1">
-        <v>44113</v>
+        <v>44114</v>
       </c>
       <c r="B72">
         <v>0.13</v>
@@ -969,7 +977,7 @@
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A73" s="1">
-        <v>44114</v>
+        <v>44115</v>
       </c>
       <c r="B73">
         <v>0.13</v>
@@ -977,7 +985,7 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A74" s="1">
-        <v>44115</v>
+        <v>44116</v>
       </c>
       <c r="B74">
         <v>0.13</v>
@@ -985,7 +993,7 @@
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A75" s="1">
-        <v>44116</v>
+        <v>44117</v>
       </c>
       <c r="B75">
         <v>0.13</v>
@@ -993,7 +1001,7 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A76" s="1">
-        <v>44117</v>
+        <v>44118</v>
       </c>
       <c r="B76">
         <v>0.13</v>
@@ -1001,7 +1009,7 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A77" s="1">
-        <v>44118</v>
+        <v>44119</v>
       </c>
       <c r="B77">
         <v>0.13</v>
@@ -1009,15 +1017,15 @@
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A78" s="1">
-        <v>44119</v>
+        <v>44120</v>
       </c>
       <c r="B78">
-        <v>0.13</v>
+        <v>0.14000000000000001</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A79" s="1">
-        <v>44120</v>
+        <v>44121</v>
       </c>
       <c r="B79">
         <v>0.14000000000000001</v>
@@ -1025,15 +1033,15 @@
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A80" s="1">
-        <v>44121</v>
+        <v>44122</v>
       </c>
       <c r="B80">
-        <v>0.14000000000000001</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A81" s="1">
-        <v>44122</v>
+        <v>44123</v>
       </c>
       <c r="B81">
         <v>0.13</v>
@@ -1041,7 +1049,7 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A82" s="1">
-        <v>44123</v>
+        <v>44124</v>
       </c>
       <c r="B82">
         <v>0.13</v>
@@ -1049,7 +1057,7 @@
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A83" s="1">
-        <v>44124</v>
+        <v>44125</v>
       </c>
       <c r="B83">
         <v>0.13</v>
@@ -1057,7 +1065,7 @@
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A84" s="1">
-        <v>44125</v>
+        <v>44126</v>
       </c>
       <c r="B84">
         <v>0.13</v>
@@ -1065,15 +1073,15 @@
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A85" s="1">
-        <v>44126</v>
+        <v>44127</v>
       </c>
       <c r="B85">
-        <v>0.13</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A86" s="1">
-        <v>44127</v>
+        <v>44128</v>
       </c>
       <c r="B86">
         <v>0.12</v>
@@ -1081,7 +1089,7 @@
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A87" s="1">
-        <v>44128</v>
+        <v>44129</v>
       </c>
       <c r="B87">
         <v>0.12</v>
@@ -1089,7 +1097,7 @@
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A88" s="1">
-        <v>44129</v>
+        <v>44130</v>
       </c>
       <c r="B88">
         <v>0.12</v>
@@ -1097,15 +1105,15 @@
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A89" s="1">
-        <v>44130</v>
+        <v>44131</v>
       </c>
       <c r="B89">
-        <v>0.12</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A90" s="1">
-        <v>44131</v>
+        <v>44132</v>
       </c>
       <c r="B90">
         <v>0.13</v>
@@ -1113,7 +1121,7 @@
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A91" s="1">
-        <v>44132</v>
+        <v>44133</v>
       </c>
       <c r="B91">
         <v>0.13</v>
@@ -1121,15 +1129,15 @@
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A92" s="1">
-        <v>44133</v>
+        <v>44134</v>
       </c>
       <c r="B92">
-        <v>0.13</v>
+        <v>0.14000000000000001</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A93" s="1">
-        <v>44134</v>
+        <v>44135</v>
       </c>
       <c r="B93">
         <v>0.14000000000000001</v>
@@ -1137,7 +1145,7 @@
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A94" s="1">
-        <v>44135</v>
+        <v>44136</v>
       </c>
       <c r="B94">
         <v>0.14000000000000001</v>
@@ -1145,7 +1153,7 @@
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A95" s="1">
-        <v>44136</v>
+        <v>44137</v>
       </c>
       <c r="B95">
         <v>0.14000000000000001</v>
@@ -1153,7 +1161,7 @@
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A96" s="1">
-        <v>44137</v>
+        <v>44138</v>
       </c>
       <c r="B96">
         <v>0.14000000000000001</v>
@@ -1161,7 +1169,7 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A97" s="1">
-        <v>44138</v>
+        <v>44139</v>
       </c>
       <c r="B97">
         <v>0.14000000000000001</v>
@@ -1169,7 +1177,7 @@
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A98" s="1">
-        <v>44139</v>
+        <v>44140</v>
       </c>
       <c r="B98">
         <v>0.14000000000000001</v>
@@ -1177,7 +1185,7 @@
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A99" s="1">
-        <v>44140</v>
+        <v>44141</v>
       </c>
       <c r="B99">
         <v>0.14000000000000001</v>
@@ -1185,47 +1193,47 @@
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A100" s="1">
-        <v>44141</v>
+        <v>44142</v>
       </c>
       <c r="B100">
-        <v>0.14000000000000001</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A101" s="1">
-        <v>44142</v>
+        <v>44143</v>
       </c>
       <c r="B101">
-        <v>0.15</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A102" s="1">
-        <v>44143</v>
+        <v>44144</v>
       </c>
       <c r="B102">
-        <v>0.17</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A103" s="1">
-        <v>44144</v>
+        <v>44145</v>
       </c>
       <c r="B103">
-        <v>0.18</v>
+        <v>0.19</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A104" s="1">
-        <v>44145</v>
+        <v>44146</v>
       </c>
       <c r="B104">
-        <v>0.19</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A105" s="1">
-        <v>44146</v>
+        <v>44147</v>
       </c>
       <c r="B105">
         <v>0.2</v>
@@ -1233,15 +1241,15 @@
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A106" s="1">
-        <v>44147</v>
+        <v>44148</v>
       </c>
       <c r="B106">
-        <v>0.2</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A107" s="1">
-        <v>44148</v>
+        <v>44149</v>
       </c>
       <c r="B107">
         <v>0.21</v>
@@ -1249,7 +1257,7 @@
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A108" s="1">
-        <v>44149</v>
+        <v>44150</v>
       </c>
       <c r="B108">
         <v>0.21</v>
@@ -1257,7 +1265,7 @@
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A109" s="1">
-        <v>44150</v>
+        <v>44151</v>
       </c>
       <c r="B109">
         <v>0.21</v>
@@ -1265,23 +1273,23 @@
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A110" s="1">
-        <v>44151</v>
+        <v>44152</v>
       </c>
       <c r="B110">
-        <v>0.21</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A111" s="1">
-        <v>44152</v>
+        <v>44153</v>
       </c>
       <c r="B111">
-        <v>0.2</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A112" s="1">
-        <v>44153</v>
+        <v>44154</v>
       </c>
       <c r="B112">
         <v>0.21</v>
@@ -1289,15 +1297,15 @@
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A113" s="1">
-        <v>44154</v>
+        <v>44155</v>
       </c>
       <c r="B113">
-        <v>0.21</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A114" s="1">
-        <v>44155</v>
+        <v>44156</v>
       </c>
       <c r="B114">
         <v>0.2</v>
@@ -1305,7 +1313,7 @@
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A115" s="1">
-        <v>44156</v>
+        <v>44157</v>
       </c>
       <c r="B115">
         <v>0.2</v>
@@ -1313,7 +1321,7 @@
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A116" s="1">
-        <v>44157</v>
+        <v>44158</v>
       </c>
       <c r="B116">
         <v>0.2</v>
@@ -1321,7 +1329,7 @@
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A117" s="1">
-        <v>44158</v>
+        <v>44159</v>
       </c>
       <c r="B117">
         <v>0.2</v>
@@ -1329,7 +1337,7 @@
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A118" s="1">
-        <v>44159</v>
+        <v>44160</v>
       </c>
       <c r="B118">
         <v>0.2</v>
@@ -1337,7 +1345,7 @@
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A119" s="1">
-        <v>44160</v>
+        <v>44161</v>
       </c>
       <c r="B119">
         <v>0.2</v>
@@ -1345,7 +1353,7 @@
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A120" s="1">
-        <v>44161</v>
+        <v>44162</v>
       </c>
       <c r="B120">
         <v>0.2</v>
@@ -1353,23 +1361,23 @@
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A121" s="1">
-        <v>44162</v>
+        <v>44163</v>
       </c>
       <c r="B121">
-        <v>0.2</v>
+        <v>0.19</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A122" s="1">
-        <v>44163</v>
+        <v>44164</v>
       </c>
       <c r="B122">
-        <v>0.19</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A123" s="1">
-        <v>44164</v>
+        <v>44165</v>
       </c>
       <c r="B123">
         <v>0.2</v>
@@ -1377,23 +1385,23 @@
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A124" s="1">
-        <v>44165</v>
+        <v>44166</v>
       </c>
       <c r="B124">
-        <v>0.2</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A125" s="1">
-        <v>44166</v>
+        <v>44167</v>
       </c>
       <c r="B125">
-        <v>0.21</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A126" s="1">
-        <v>44167</v>
+        <v>44168</v>
       </c>
       <c r="B126">
         <v>0.22</v>
@@ -1401,23 +1409,23 @@
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A127" s="1">
-        <v>44168</v>
+        <v>44169</v>
       </c>
       <c r="B127">
-        <v>0.22</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A128" s="1">
-        <v>44169</v>
+        <v>44170</v>
       </c>
       <c r="B128">
-        <v>0.24</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A129" s="1">
-        <v>44170</v>
+        <v>44171</v>
       </c>
       <c r="B129">
         <v>0.25</v>
@@ -1425,7 +1433,7 @@
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A130" s="1">
-        <v>44171</v>
+        <v>44172</v>
       </c>
       <c r="B130">
         <v>0.25</v>
@@ -1433,7 +1441,7 @@
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A131" s="1">
-        <v>44172</v>
+        <v>44173</v>
       </c>
       <c r="B131">
         <v>0.25</v>
@@ -1441,15 +1449,15 @@
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A132" s="1">
-        <v>44173</v>
+        <v>44174</v>
       </c>
       <c r="B132">
-        <v>0.25</v>
+        <v>0.26</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A133" s="1">
-        <v>44174</v>
+        <v>44175</v>
       </c>
       <c r="B133">
         <v>0.26</v>
@@ -1457,7 +1465,7 @@
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A134" s="1">
-        <v>44175</v>
+        <v>44176</v>
       </c>
       <c r="B134">
         <v>0.26</v>
@@ -1465,7 +1473,7 @@
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A135" s="1">
-        <v>44176</v>
+        <v>44177</v>
       </c>
       <c r="B135">
         <v>0.26</v>
@@ -1473,7 +1481,7 @@
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A136" s="1">
-        <v>44177</v>
+        <v>44178</v>
       </c>
       <c r="B136">
         <v>0.26</v>
@@ -1481,7 +1489,7 @@
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A137" s="1">
-        <v>44178</v>
+        <v>44179</v>
       </c>
       <c r="B137">
         <v>0.26</v>
@@ -1489,7 +1497,7 @@
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A138" s="1">
-        <v>44179</v>
+        <v>44180</v>
       </c>
       <c r="B138">
         <v>0.26</v>
@@ -1497,7 +1505,7 @@
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A139" s="1">
-        <v>44180</v>
+        <v>44181</v>
       </c>
       <c r="B139">
         <v>0.26</v>
@@ -1505,15 +1513,15 @@
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A140" s="1">
-        <v>44181</v>
+        <v>44182</v>
       </c>
       <c r="B140">
-        <v>0.26</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A141" s="1">
-        <v>44182</v>
+        <v>44183</v>
       </c>
       <c r="B141">
         <v>0.25</v>
@@ -1521,7 +1529,7 @@
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A142" s="1">
-        <v>44183</v>
+        <v>44184</v>
       </c>
       <c r="B142">
         <v>0.25</v>
@@ -1529,15 +1537,15 @@
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A143" s="1">
-        <v>44184</v>
+        <v>44185</v>
       </c>
       <c r="B143">
-        <v>0.25</v>
+        <v>0.26</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A144" s="1">
-        <v>44185</v>
+        <v>44186</v>
       </c>
       <c r="B144">
         <v>0.26</v>
@@ -1545,7 +1553,7 @@
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A145" s="1">
-        <v>44186</v>
+        <v>44187</v>
       </c>
       <c r="B145">
         <v>0.26</v>
@@ -1553,7 +1561,7 @@
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A146" s="1">
-        <v>44187</v>
+        <v>44188</v>
       </c>
       <c r="B146">
         <v>0.26</v>
@@ -1561,31 +1569,31 @@
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A147" s="1">
-        <v>44188</v>
+        <v>44189</v>
       </c>
       <c r="B147">
-        <v>0.26</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A148" s="1">
-        <v>44189</v>
+        <v>44190</v>
       </c>
       <c r="B148">
-        <v>0.25</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A149" s="1">
-        <v>44190</v>
+        <v>44191</v>
       </c>
       <c r="B149">
-        <v>0.24</v>
+        <v>0.23</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A150" s="1">
-        <v>44191</v>
+        <v>44192</v>
       </c>
       <c r="B150">
         <v>0.23</v>
@@ -1593,7 +1601,7 @@
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A151" s="1">
-        <v>44192</v>
+        <v>44193</v>
       </c>
       <c r="B151">
         <v>0.23</v>
@@ -1601,47 +1609,47 @@
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A152" s="1">
-        <v>44193</v>
+        <v>44194</v>
       </c>
       <c r="B152">
-        <v>0.23</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A153" s="1">
-        <v>44194</v>
+        <v>44195</v>
       </c>
       <c r="B153">
-        <v>0.22</v>
+        <v>0.23</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A154" s="1">
-        <v>44195</v>
+        <v>44196</v>
       </c>
       <c r="B154">
-        <v>0.23</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A155" s="1">
-        <v>44196</v>
+        <v>44197</v>
       </c>
       <c r="B155">
-        <v>0.24</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A156" s="1">
-        <v>44197</v>
+        <v>44198</v>
       </c>
       <c r="B156">
-        <v>0.25</v>
+        <v>0.26</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A157" s="1">
-        <v>44198</v>
+        <v>44199</v>
       </c>
       <c r="B157">
         <v>0.26</v>
@@ -1649,15 +1657,15 @@
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A158" s="1">
-        <v>44199</v>
+        <v>44200</v>
       </c>
       <c r="B158">
-        <v>0.26</v>
+        <v>0.27</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A159" s="1">
-        <v>44200</v>
+        <v>44201</v>
       </c>
       <c r="B159">
         <v>0.27</v>
@@ -1665,15 +1673,15 @@
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A160" s="1">
-        <v>44201</v>
+        <v>44202</v>
       </c>
       <c r="B160">
-        <v>0.27</v>
+        <v>0.28000000000000003</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A161" s="1">
-        <v>44202</v>
+        <v>44203</v>
       </c>
       <c r="B161">
         <v>0.28000000000000003</v>
@@ -1681,23 +1689,23 @@
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A162" s="1">
-        <v>44203</v>
+        <v>44204</v>
       </c>
       <c r="B162">
-        <v>0.28000000000000003</v>
+        <v>0.28999999999999998</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A163" s="1">
-        <v>44204</v>
+        <v>44205</v>
       </c>
       <c r="B163">
-        <v>0.28999999999999998</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A164" s="1">
-        <v>44205</v>
+        <v>44206</v>
       </c>
       <c r="B164">
         <v>0.3</v>
@@ -1705,15 +1713,15 @@
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A165" s="1">
-        <v>44206</v>
+        <v>44207</v>
       </c>
       <c r="B165">
-        <v>0.3</v>
+        <v>0.28999999999999998</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A166" s="1">
-        <v>44207</v>
+        <v>44208</v>
       </c>
       <c r="B166">
         <v>0.28999999999999998</v>
@@ -1721,15 +1729,15 @@
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A167" s="1">
-        <v>44208</v>
+        <v>44209</v>
       </c>
       <c r="B167">
-        <v>0.28999999999999998</v>
+        <v>0.28000000000000003</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A168" s="1">
-        <v>44209</v>
+        <v>44210</v>
       </c>
       <c r="B168">
         <v>0.28000000000000003</v>
@@ -1737,15 +1745,15 @@
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A169" s="1">
-        <v>44210</v>
+        <v>44211</v>
       </c>
       <c r="B169">
-        <v>0.28000000000000003</v>
+        <v>0.27</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A170" s="1">
-        <v>44211</v>
+        <v>44212</v>
       </c>
       <c r="B170">
         <v>0.27</v>
@@ -1753,7 +1761,7 @@
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A171" s="1">
-        <v>44212</v>
+        <v>44213</v>
       </c>
       <c r="B171">
         <v>0.27</v>
@@ -1761,7 +1769,7 @@
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A172" s="1">
-        <v>44213</v>
+        <v>44214</v>
       </c>
       <c r="B172">
         <v>0.27</v>
@@ -1769,23 +1777,23 @@
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A173" s="1">
-        <v>44214</v>
+        <v>44215</v>
       </c>
       <c r="B173">
-        <v>0.27</v>
+        <v>0.28000000000000003</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A174" s="1">
-        <v>44215</v>
+        <v>44216</v>
       </c>
       <c r="B174">
-        <v>0.28000000000000003</v>
+        <v>0.27</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A175" s="1">
-        <v>44216</v>
+        <v>44217</v>
       </c>
       <c r="B175">
         <v>0.27</v>
@@ -1793,7 +1801,7 @@
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A176" s="1">
-        <v>44217</v>
+        <v>44218</v>
       </c>
       <c r="B176">
         <v>0.27</v>
@@ -1801,7 +1809,7 @@
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A177" s="1">
-        <v>44218</v>
+        <v>44219</v>
       </c>
       <c r="B177">
         <v>0.27</v>
@@ -1809,7 +1817,7 @@
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A178" s="1">
-        <v>44219</v>
+        <v>44220</v>
       </c>
       <c r="B178">
         <v>0.27</v>
@@ -1817,15 +1825,15 @@
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A179" s="1">
-        <v>44220</v>
+        <v>44221</v>
       </c>
       <c r="B179">
-        <v>0.27</v>
+        <v>0.28000000000000003</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A180" s="1">
-        <v>44221</v>
+        <v>44222</v>
       </c>
       <c r="B180">
         <v>0.28000000000000003</v>
@@ -1833,7 +1841,7 @@
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A181" s="1">
-        <v>44222</v>
+        <v>44223</v>
       </c>
       <c r="B181">
         <v>0.28000000000000003</v>
@@ -1841,7 +1849,7 @@
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A182" s="1">
-        <v>44223</v>
+        <v>44224</v>
       </c>
       <c r="B182">
         <v>0.28000000000000003</v>
@@ -1849,7 +1857,7 @@
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A183" s="1">
-        <v>44224</v>
+        <v>44225</v>
       </c>
       <c r="B183">
         <v>0.28000000000000003</v>
@@ -1857,7 +1865,7 @@
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A184" s="1">
-        <v>44225</v>
+        <v>44226</v>
       </c>
       <c r="B184">
         <v>0.28000000000000003</v>
@@ -1865,7 +1873,7 @@
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A185" s="1">
-        <v>44226</v>
+        <v>44227</v>
       </c>
       <c r="B185">
         <v>0.28000000000000003</v>
@@ -1873,15 +1881,15 @@
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A186" s="1">
-        <v>44227</v>
+        <v>44228</v>
       </c>
       <c r="B186">
-        <v>0.28000000000000003</v>
+        <v>0.27</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A187" s="1">
-        <v>44228</v>
+        <v>44229</v>
       </c>
       <c r="B187">
         <v>0.27</v>
@@ -1889,23 +1897,23 @@
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A188" s="1">
-        <v>44229</v>
+        <v>44230</v>
       </c>
       <c r="B188">
-        <v>0.27</v>
+        <v>0.26</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A189" s="1">
-        <v>44230</v>
+        <v>44231</v>
       </c>
       <c r="B189">
-        <v>0.26</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A190" s="1">
-        <v>44231</v>
+        <v>44232</v>
       </c>
       <c r="B190">
         <v>0.25</v>
@@ -1913,15 +1921,15 @@
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A191" s="1">
-        <v>44232</v>
+        <v>44233</v>
       </c>
       <c r="B191">
-        <v>0.25</v>
+        <v>0.26</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A192" s="1">
-        <v>44233</v>
+        <v>44234</v>
       </c>
       <c r="B192">
         <v>0.26</v>
@@ -1929,7 +1937,7 @@
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A193" s="1">
-        <v>44234</v>
+        <v>44235</v>
       </c>
       <c r="B193">
         <v>0.26</v>
@@ -1937,31 +1945,31 @@
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A194" s="1">
-        <v>44235</v>
+        <v>44236</v>
       </c>
       <c r="B194">
-        <v>0.26</v>
+        <v>0.27</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A195" s="1">
-        <v>44236</v>
+        <v>44237</v>
       </c>
       <c r="B195">
-        <v>0.27</v>
+        <v>0.26</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A196" s="1">
-        <v>44237</v>
+        <v>44238</v>
       </c>
       <c r="B196">
-        <v>0.26</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A197" s="1">
-        <v>44238</v>
+        <v>44239</v>
       </c>
       <c r="B197">
         <v>0.25</v>
@@ -1969,39 +1977,39 @@
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A198" s="1">
-        <v>44239</v>
+        <v>44240</v>
       </c>
       <c r="B198">
-        <v>0.25</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A199" s="1">
-        <v>44240</v>
+        <v>44241</v>
       </c>
       <c r="B199">
-        <v>0.24</v>
+        <v>0.23</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A200" s="1">
-        <v>44241</v>
+        <v>44242</v>
       </c>
       <c r="B200">
-        <v>0.23</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A201" s="1">
-        <v>44242</v>
+        <v>44243</v>
       </c>
       <c r="B201">
-        <v>0.22</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A202" s="1">
-        <v>44243</v>
+        <v>44244</v>
       </c>
       <c r="B202">
         <v>0.21</v>
@@ -2009,7 +2017,7 @@
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A203" s="1">
-        <v>44244</v>
+        <v>44245</v>
       </c>
       <c r="B203">
         <v>0.21</v>
@@ -2017,15 +2025,15 @@
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A204" s="1">
-        <v>44245</v>
+        <v>44246</v>
       </c>
       <c r="B204">
-        <v>0.21</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A205" s="1">
-        <v>44246</v>
+        <v>44247</v>
       </c>
       <c r="B205">
         <v>0.2</v>
@@ -2033,23 +2041,23 @@
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A206" s="1">
-        <v>44247</v>
+        <v>44248</v>
       </c>
       <c r="B206">
-        <v>0.2</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A207" s="1">
-        <v>44248</v>
+        <v>44249</v>
       </c>
       <c r="B207">
-        <v>0.21</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A208" s="1">
-        <v>44249</v>
+        <v>44250</v>
       </c>
       <c r="B208">
         <v>0.2</v>
@@ -2057,23 +2065,23 @@
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A209" s="1">
-        <v>44250</v>
+        <v>44251</v>
       </c>
       <c r="B209">
-        <v>0.2</v>
+        <v>0.19</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A210" s="1">
-        <v>44251</v>
+        <v>44252</v>
       </c>
       <c r="B210">
-        <v>0.19</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A211" s="1">
-        <v>44252</v>
+        <v>44253</v>
       </c>
       <c r="B211">
         <v>0.18</v>
@@ -2081,31 +2089,31 @@
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A212" s="1">
-        <v>44253</v>
+        <v>44254</v>
       </c>
       <c r="B212">
-        <v>0.18</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A213" s="1">
-        <v>44254</v>
+        <v>44255</v>
       </c>
       <c r="B213">
-        <v>0.17</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A214" s="1">
-        <v>44255</v>
+        <v>44256</v>
       </c>
       <c r="B214">
-        <v>0.16</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A215" s="1">
-        <v>44256</v>
+        <v>44257</v>
       </c>
       <c r="B215">
         <v>0.17</v>
@@ -2113,23 +2121,23 @@
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A216" s="1">
-        <v>44257</v>
+        <v>44258</v>
       </c>
       <c r="B216">
-        <v>0.17</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A217" s="1">
-        <v>44258</v>
+        <v>44259</v>
       </c>
       <c r="B217">
-        <v>0.16</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A218" s="1">
-        <v>44259</v>
+        <v>44260</v>
       </c>
       <c r="B218">
         <v>0.17</v>
@@ -2137,15 +2145,15 @@
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A219" s="1">
-        <v>44260</v>
+        <v>44261</v>
       </c>
       <c r="B219">
-        <v>0.17</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A220" s="1">
-        <v>44261</v>
+        <v>44262</v>
       </c>
       <c r="B220">
         <v>0.16</v>
@@ -2153,7 +2161,7 @@
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A221" s="1">
-        <v>44262</v>
+        <v>44263</v>
       </c>
       <c r="B221">
         <v>0.16</v>
@@ -2161,7 +2169,7 @@
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A222" s="1">
-        <v>44263</v>
+        <v>44264</v>
       </c>
       <c r="B222">
         <v>0.16</v>
@@ -2169,7 +2177,7 @@
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A223" s="1">
-        <v>44264</v>
+        <v>44265</v>
       </c>
       <c r="B223">
         <v>0.16</v>
@@ -2177,7 +2185,7 @@
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A224" s="1">
-        <v>44265</v>
+        <v>44266</v>
       </c>
       <c r="B224">
         <v>0.16</v>
@@ -2185,7 +2193,7 @@
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A225" s="1">
-        <v>44266</v>
+        <v>44267</v>
       </c>
       <c r="B225">
         <v>0.16</v>
@@ -2193,7 +2201,7 @@
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A226" s="1">
-        <v>44267</v>
+        <v>44268</v>
       </c>
       <c r="B226">
         <v>0.16</v>
@@ -2201,7 +2209,7 @@
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A227" s="1">
-        <v>44268</v>
+        <v>44269</v>
       </c>
       <c r="B227">
         <v>0.16</v>
@@ -2209,7 +2217,7 @@
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A228" s="1">
-        <v>44269</v>
+        <v>44270</v>
       </c>
       <c r="B228">
         <v>0.16</v>
@@ -2217,7 +2225,7 @@
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A229" s="1">
-        <v>44270</v>
+        <v>44271</v>
       </c>
       <c r="B229">
         <v>0.16</v>
@@ -2225,15 +2233,15 @@
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A230" s="1">
-        <v>44271</v>
+        <v>44272</v>
       </c>
       <c r="B230">
-        <v>0.16</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A231" s="1">
-        <v>44272</v>
+        <v>44273</v>
       </c>
       <c r="B231">
         <v>0.15</v>
@@ -2241,7 +2249,7 @@
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A232" s="1">
-        <v>44273</v>
+        <v>44274</v>
       </c>
       <c r="B232">
         <v>0.15</v>
@@ -2249,7 +2257,7 @@
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A233" s="1">
-        <v>44274</v>
+        <v>44275</v>
       </c>
       <c r="B233">
         <v>0.15</v>
@@ -2257,7 +2265,7 @@
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A234" s="1">
-        <v>44275</v>
+        <v>44276</v>
       </c>
       <c r="B234">
         <v>0.15</v>
@@ -2265,7 +2273,7 @@
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A235" s="1">
-        <v>44276</v>
+        <v>44277</v>
       </c>
       <c r="B235">
         <v>0.15</v>
@@ -2273,7 +2281,7 @@
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A236" s="1">
-        <v>44277</v>
+        <v>44278</v>
       </c>
       <c r="B236">
         <v>0.15</v>
@@ -2281,15 +2289,15 @@
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A237" s="1">
-        <v>44278</v>
+        <v>44279</v>
       </c>
       <c r="B237">
-        <v>0.15</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A238" s="1">
-        <v>44279</v>
+        <v>44280</v>
       </c>
       <c r="B238">
         <v>0.16</v>
@@ -2297,7 +2305,7 @@
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A239" s="1">
-        <v>44280</v>
+        <v>44281</v>
       </c>
       <c r="B239">
         <v>0.16</v>
@@ -2305,7 +2313,7 @@
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A240" s="1">
-        <v>44281</v>
+        <v>44282</v>
       </c>
       <c r="B240">
         <v>0.16</v>
@@ -2313,23 +2321,23 @@
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A241" s="1">
-        <v>44282</v>
+        <v>44283</v>
       </c>
       <c r="B241">
-        <v>0.16</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A242" s="1">
-        <v>44283</v>
+        <v>44284</v>
       </c>
       <c r="B242">
-        <v>0.17</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A243" s="1">
-        <v>44284</v>
+        <v>44285</v>
       </c>
       <c r="B243">
         <v>0.16</v>
@@ -2337,7 +2345,7 @@
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A244" s="1">
-        <v>44285</v>
+        <v>44286</v>
       </c>
       <c r="B244">
         <v>0.16</v>
@@ -2345,7 +2353,7 @@
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A245" s="1">
-        <v>44286</v>
+        <v>44287</v>
       </c>
       <c r="B245">
         <v>0.16</v>
@@ -2353,7 +2361,7 @@
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A246" s="1">
-        <v>44287</v>
+        <v>44288</v>
       </c>
       <c r="B246">
         <v>0.16</v>
@@ -2361,7 +2369,7 @@
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A247" s="1">
-        <v>44288</v>
+        <v>44289</v>
       </c>
       <c r="B247">
         <v>0.16</v>
@@ -2369,23 +2377,23 @@
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A248" s="1">
-        <v>44289</v>
+        <v>44290</v>
       </c>
       <c r="B248">
-        <v>0.16</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A249" s="1">
-        <v>44290</v>
+        <v>44291</v>
       </c>
       <c r="B249">
-        <v>0.15</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A250" s="1">
-        <v>44291</v>
+        <v>44292</v>
       </c>
       <c r="B250">
         <v>0.16</v>
@@ -2393,7 +2401,7 @@
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A251" s="1">
-        <v>44292</v>
+        <v>44293</v>
       </c>
       <c r="B251">
         <v>0.16</v>
@@ -2401,7 +2409,7 @@
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A252" s="1">
-        <v>44293</v>
+        <v>44294</v>
       </c>
       <c r="B252">
         <v>0.16</v>
@@ -2409,7 +2417,7 @@
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A253" s="1">
-        <v>44294</v>
+        <v>44295</v>
       </c>
       <c r="B253">
         <v>0.16</v>
@@ -2417,7 +2425,7 @@
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A254" s="1">
-        <v>44295</v>
+        <v>44296</v>
       </c>
       <c r="B254">
         <v>0.16</v>
@@ -2425,7 +2433,7 @@
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A255" s="1">
-        <v>44296</v>
+        <v>44297</v>
       </c>
       <c r="B255">
         <v>0.16</v>
@@ -2433,7 +2441,7 @@
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A256" s="1">
-        <v>44297</v>
+        <v>44298</v>
       </c>
       <c r="B256">
         <v>0.16</v>
@@ -2441,7 +2449,7 @@
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A257" s="1">
-        <v>44298</v>
+        <v>44299</v>
       </c>
       <c r="B257">
         <v>0.16</v>
@@ -2449,15 +2457,15 @@
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A258" s="1">
-        <v>44299</v>
+        <v>44300</v>
       </c>
       <c r="B258">
-        <v>0.16</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A259" s="1">
-        <v>44300</v>
+        <v>44301</v>
       </c>
       <c r="B259">
         <v>0.17</v>
@@ -2465,7 +2473,7 @@
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A260" s="1">
-        <v>44301</v>
+        <v>44302</v>
       </c>
       <c r="B260">
         <v>0.17</v>
@@ -2473,15 +2481,15 @@
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A261" s="1">
-        <v>44302</v>
+        <v>44303</v>
       </c>
       <c r="B261">
-        <v>0.17</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A262" s="1">
-        <v>44303</v>
+        <v>44304</v>
       </c>
       <c r="B262">
         <v>0.18</v>
@@ -2489,7 +2497,7 @@
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A263" s="1">
-        <v>44304</v>
+        <v>44305</v>
       </c>
       <c r="B263">
         <v>0.18</v>
@@ -2497,7 +2505,7 @@
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A264" s="1">
-        <v>44305</v>
+        <v>44306</v>
       </c>
       <c r="B264">
         <v>0.18</v>
@@ -2505,23 +2513,23 @@
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A265" s="1">
-        <v>44306</v>
+        <v>44307</v>
       </c>
       <c r="B265">
-        <v>0.18</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A266" s="1">
-        <v>44307</v>
+        <v>44308</v>
       </c>
       <c r="B266">
-        <v>0.17</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A267" s="1">
-        <v>44308</v>
+        <v>44309</v>
       </c>
       <c r="B267">
         <v>0.18</v>
@@ -2529,7 +2537,7 @@
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A268" s="1">
-        <v>44309</v>
+        <v>44310</v>
       </c>
       <c r="B268">
         <v>0.18</v>
@@ -2537,7 +2545,7 @@
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A269" s="1">
-        <v>44310</v>
+        <v>44311</v>
       </c>
       <c r="B269">
         <v>0.18</v>
@@ -2545,7 +2553,7 @@
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A270" s="1">
-        <v>44311</v>
+        <v>44312</v>
       </c>
       <c r="B270">
         <v>0.18</v>
@@ -2553,7 +2561,7 @@
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A271" s="1">
-        <v>44312</v>
+        <v>44313</v>
       </c>
       <c r="B271">
         <v>0.18</v>
@@ -2561,7 +2569,7 @@
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A272" s="1">
-        <v>44313</v>
+        <v>44314</v>
       </c>
       <c r="B272">
         <v>0.18</v>
@@ -2569,7 +2577,7 @@
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A273" s="1">
-        <v>44314</v>
+        <v>44315</v>
       </c>
       <c r="B273">
         <v>0.18</v>
@@ -2577,7 +2585,7 @@
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A274" s="1">
-        <v>44315</v>
+        <v>44316</v>
       </c>
       <c r="B274">
         <v>0.18</v>
@@ -2585,15 +2593,15 @@
     </row>
     <row r="275" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A275" s="1">
-        <v>44316</v>
+        <v>44317</v>
       </c>
       <c r="B275">
-        <v>0.18</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A276" s="1">
-        <v>44317</v>
+        <v>44318</v>
       </c>
       <c r="B276">
         <v>0.17</v>
@@ -2601,7 +2609,7 @@
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A277" s="1">
-        <v>44318</v>
+        <v>44319</v>
       </c>
       <c r="B277">
         <v>0.17</v>
@@ -2609,15 +2617,15 @@
     </row>
     <row r="278" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A278" s="1">
-        <v>44319</v>
+        <v>44320</v>
       </c>
       <c r="B278">
-        <v>0.17</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="279" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A279" s="1">
-        <v>44320</v>
+        <v>44321</v>
       </c>
       <c r="B279">
         <v>0.16</v>
@@ -2625,15 +2633,15 @@
     </row>
     <row r="280" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A280" s="1">
-        <v>44321</v>
+        <v>44322</v>
       </c>
       <c r="B280">
-        <v>0.16</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="281" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A281" s="1">
-        <v>44322</v>
+        <v>44323</v>
       </c>
       <c r="B281">
         <v>0.15</v>
@@ -2641,7 +2649,7 @@
     </row>
     <row r="282" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A282" s="1">
-        <v>44323</v>
+        <v>44324</v>
       </c>
       <c r="B282">
         <v>0.15</v>
@@ -2649,23 +2657,23 @@
     </row>
     <row r="283" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A283" s="1">
-        <v>44324</v>
+        <v>44325</v>
       </c>
       <c r="B283">
-        <v>0.15</v>
+        <v>0.14000000000000001</v>
       </c>
     </row>
     <row r="284" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A284" s="1">
-        <v>44325</v>
+        <v>44326</v>
       </c>
       <c r="B284">
-        <v>0.14000000000000001</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="285" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A285" s="1">
-        <v>44326</v>
+        <v>44327</v>
       </c>
       <c r="B285">
         <v>0.15</v>
@@ -2673,7 +2681,7 @@
     </row>
     <row r="286" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A286" s="1">
-        <v>44327</v>
+        <v>44328</v>
       </c>
       <c r="B286">
         <v>0.15</v>
@@ -2681,7 +2689,7 @@
     </row>
     <row r="287" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A287" s="1">
-        <v>44328</v>
+        <v>44329</v>
       </c>
       <c r="B287">
         <v>0.15</v>
@@ -2689,15 +2697,15 @@
     </row>
     <row r="288" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A288" s="1">
-        <v>44329</v>
+        <v>44330</v>
       </c>
       <c r="B288">
-        <v>0.15</v>
+        <v>0.14000000000000001</v>
       </c>
     </row>
     <row r="289" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A289" s="1">
-        <v>44330</v>
+        <v>44331</v>
       </c>
       <c r="B289">
         <v>0.14000000000000001</v>
@@ -2705,7 +2713,7 @@
     </row>
     <row r="290" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A290" s="1">
-        <v>44331</v>
+        <v>44332</v>
       </c>
       <c r="B290">
         <v>0.14000000000000001</v>
@@ -2713,15 +2721,15 @@
     </row>
     <row r="291" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A291" s="1">
-        <v>44332</v>
+        <v>44333</v>
       </c>
       <c r="B291">
-        <v>0.14000000000000001</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="292" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A292" s="1">
-        <v>44333</v>
+        <v>44334</v>
       </c>
       <c r="B292">
         <v>0.13</v>
@@ -2729,7 +2737,7 @@
     </row>
     <row r="293" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A293" s="1">
-        <v>44334</v>
+        <v>44335</v>
       </c>
       <c r="B293">
         <v>0.13</v>
@@ -2737,7 +2745,7 @@
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A294" s="1">
-        <v>44335</v>
+        <v>44336</v>
       </c>
       <c r="B294">
         <v>0.13</v>
@@ -2745,23 +2753,23 @@
     </row>
     <row r="295" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A295" s="1">
-        <v>44336</v>
+        <v>44337</v>
       </c>
       <c r="B295">
-        <v>0.13</v>
+        <v>0.14000000000000001</v>
       </c>
     </row>
     <row r="296" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A296" s="1">
-        <v>44337</v>
+        <v>44338</v>
       </c>
       <c r="B296">
-        <v>0.14000000000000001</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="297" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A297" s="1">
-        <v>44338</v>
+        <v>44339</v>
       </c>
       <c r="B297">
         <v>0.13</v>
@@ -2769,7 +2777,7 @@
     </row>
     <row r="298" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A298" s="1">
-        <v>44339</v>
+        <v>44340</v>
       </c>
       <c r="B298">
         <v>0.13</v>
@@ -2777,7 +2785,7 @@
     </row>
     <row r="299" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A299" s="1">
-        <v>44340</v>
+        <v>44341</v>
       </c>
       <c r="B299">
         <v>0.13</v>
@@ -2785,7 +2793,7 @@
     </row>
     <row r="300" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A300" s="1">
-        <v>44341</v>
+        <v>44342</v>
       </c>
       <c r="B300">
         <v>0.13</v>
@@ -2793,7 +2801,7 @@
     </row>
     <row r="301" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A301" s="1">
-        <v>44342</v>
+        <v>44343</v>
       </c>
       <c r="B301">
         <v>0.13</v>
@@ -2801,7 +2809,7 @@
     </row>
     <row r="302" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A302" s="1">
-        <v>44343</v>
+        <v>44344</v>
       </c>
       <c r="B302">
         <v>0.13</v>
@@ -2809,15 +2817,15 @@
     </row>
     <row r="303" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A303" s="1">
-        <v>44344</v>
+        <v>44345</v>
       </c>
       <c r="B303">
-        <v>0.13</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="304" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A304" s="1">
-        <v>44345</v>
+        <v>44346</v>
       </c>
       <c r="B304">
         <v>0.12</v>
@@ -2825,7 +2833,7 @@
     </row>
     <row r="305" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A305" s="1">
-        <v>44346</v>
+        <v>44347</v>
       </c>
       <c r="B305">
         <v>0.12</v>
@@ -2833,15 +2841,15 @@
     </row>
     <row r="306" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A306" s="1">
-        <v>44347</v>
+        <v>44348</v>
       </c>
       <c r="B306">
-        <v>0.12</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="307" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A307" s="1">
-        <v>44348</v>
+        <v>44349</v>
       </c>
       <c r="B307">
         <v>0.11</v>
@@ -2849,7 +2857,7 @@
     </row>
     <row r="308" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A308" s="1">
-        <v>44349</v>
+        <v>44350</v>
       </c>
       <c r="B308">
         <v>0.11</v>
@@ -2857,7 +2865,7 @@
     </row>
     <row r="309" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A309" s="1">
-        <v>44350</v>
+        <v>44351</v>
       </c>
       <c r="B309">
         <v>0.11</v>
@@ -2865,7 +2873,7 @@
     </row>
     <row r="310" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A310" s="1">
-        <v>44351</v>
+        <v>44352</v>
       </c>
       <c r="B310">
         <v>0.11</v>
@@ -2873,7 +2881,7 @@
     </row>
     <row r="311" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A311" s="1">
-        <v>44352</v>
+        <v>44353</v>
       </c>
       <c r="B311">
         <v>0.11</v>
@@ -2881,7 +2889,7 @@
     </row>
     <row r="312" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A312" s="1">
-        <v>44353</v>
+        <v>44354</v>
       </c>
       <c r="B312">
         <v>0.11</v>
@@ -2889,7 +2897,7 @@
     </row>
     <row r="313" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A313" s="1">
-        <v>44354</v>
+        <v>44355</v>
       </c>
       <c r="B313">
         <v>0.11</v>
@@ -2897,7 +2905,7 @@
     </row>
     <row r="314" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A314" s="1">
-        <v>44355</v>
+        <v>44356</v>
       </c>
       <c r="B314">
         <v>0.11</v>
@@ -2905,23 +2913,23 @@
     </row>
     <row r="315" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A315" s="1">
-        <v>44356</v>
+        <v>44357</v>
       </c>
       <c r="B315">
-        <v>0.11</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="316" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A316" s="1">
-        <v>44357</v>
+        <v>44358</v>
       </c>
       <c r="B316">
-        <v>0.1</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="317" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A317" s="1">
-        <v>44358</v>
+        <v>44359</v>
       </c>
       <c r="B317">
         <v>0.09</v>
@@ -2929,7 +2937,7 @@
     </row>
     <row r="318" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A318" s="1">
-        <v>44359</v>
+        <v>44360</v>
       </c>
       <c r="B318">
         <v>0.09</v>
@@ -2937,7 +2945,7 @@
     </row>
     <row r="319" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A319" s="1">
-        <v>44360</v>
+        <v>44361</v>
       </c>
       <c r="B319">
         <v>0.09</v>
@@ -2945,7 +2953,7 @@
     </row>
     <row r="320" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A320" s="1">
-        <v>44361</v>
+        <v>44362</v>
       </c>
       <c r="B320">
         <v>0.09</v>
@@ -2953,7 +2961,7 @@
     </row>
     <row r="321" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A321" s="1">
-        <v>44362</v>
+        <v>44363</v>
       </c>
       <c r="B321">
         <v>0.09</v>
@@ -2961,23 +2969,23 @@
     </row>
     <row r="322" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A322" s="1">
-        <v>44363</v>
+        <v>44364</v>
       </c>
       <c r="B322">
-        <v>0.09</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="323" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A323" s="1">
-        <v>44364</v>
+        <v>44365</v>
       </c>
       <c r="B323">
-        <v>0.08</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="324" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A324" s="1">
-        <v>44365</v>
+        <v>44366</v>
       </c>
       <c r="B324">
         <v>0.09</v>
@@ -2985,7 +2993,7 @@
     </row>
     <row r="325" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A325" s="1">
-        <v>44366</v>
+        <v>44367</v>
       </c>
       <c r="B325">
         <v>0.09</v>
@@ -2993,15 +3001,15 @@
     </row>
     <row r="326" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A326" s="1">
-        <v>44367</v>
+        <v>44368</v>
       </c>
       <c r="B326">
-        <v>0.09</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="327" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A327" s="1">
-        <v>44368</v>
+        <v>44369</v>
       </c>
       <c r="B327">
         <v>0.08</v>
@@ -3009,15 +3017,15 @@
     </row>
     <row r="328" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A328" s="1">
-        <v>44369</v>
+        <v>44370</v>
       </c>
       <c r="B328">
-        <v>0.08</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="329" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A329" s="1">
-        <v>44370</v>
+        <v>44371</v>
       </c>
       <c r="B329">
         <v>0.09</v>
@@ -3025,23 +3033,23 @@
     </row>
     <row r="330" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A330" s="1">
-        <v>44371</v>
+        <v>44372</v>
       </c>
       <c r="B330">
-        <v>0.09</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="331" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A331" s="1">
-        <v>44372</v>
+        <v>44373</v>
       </c>
       <c r="B331">
-        <v>0.1</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="332" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A332" s="1">
-        <v>44373</v>
+        <v>44374</v>
       </c>
       <c r="B332">
         <v>0.09</v>
@@ -3049,7 +3057,7 @@
     </row>
     <row r="333" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A333" s="1">
-        <v>44374</v>
+        <v>44375</v>
       </c>
       <c r="B333">
         <v>0.09</v>
@@ -3057,7 +3065,7 @@
     </row>
     <row r="334" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A334" s="1">
-        <v>44375</v>
+        <v>44376</v>
       </c>
       <c r="B334">
         <v>0.09</v>
@@ -3065,7 +3073,7 @@
     </row>
     <row r="335" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A335" s="1">
-        <v>44376</v>
+        <v>44377</v>
       </c>
       <c r="B335">
         <v>0.09</v>
@@ -3073,15 +3081,15 @@
     </row>
     <row r="336" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A336" s="1">
-        <v>44377</v>
+        <v>44378</v>
       </c>
       <c r="B336">
-        <v>0.09</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="337" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A337" s="1">
-        <v>44378</v>
+        <v>44379</v>
       </c>
       <c r="B337">
         <v>0.08</v>
@@ -3089,7 +3097,7 @@
     </row>
     <row r="338" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A338" s="1">
-        <v>44379</v>
+        <v>44380</v>
       </c>
       <c r="B338">
         <v>0.08</v>
@@ -3097,15 +3105,15 @@
     </row>
     <row r="339" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A339" s="1">
-        <v>44380</v>
+        <v>44381</v>
       </c>
       <c r="B339">
-        <v>0.08</v>
+        <v>7.0000000000000007E-2</v>
       </c>
     </row>
     <row r="340" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A340" s="1">
-        <v>44381</v>
+        <v>44382</v>
       </c>
       <c r="B340">
         <v>7.0000000000000007E-2</v>
@@ -3113,15 +3121,15 @@
     </row>
     <row r="341" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A341" s="1">
-        <v>44382</v>
+        <v>44383</v>
       </c>
       <c r="B341">
-        <v>7.0000000000000007E-2</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="342" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A342" s="1">
-        <v>44383</v>
+        <v>44384</v>
       </c>
       <c r="B342">
         <v>0.08</v>
@@ -3129,7 +3137,7 @@
     </row>
     <row r="343" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A343" s="1">
-        <v>44384</v>
+        <v>44385</v>
       </c>
       <c r="B343">
         <v>0.08</v>
@@ -3137,7 +3145,7 @@
     </row>
     <row r="344" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A344" s="1">
-        <v>44385</v>
+        <v>44386</v>
       </c>
       <c r="B344">
         <v>0.08</v>
@@ -3145,15 +3153,15 @@
     </row>
     <row r="345" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A345" s="1">
-        <v>44386</v>
+        <v>44387</v>
       </c>
       <c r="B345">
-        <v>0.08</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="346" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A346" s="1">
-        <v>44387</v>
+        <v>44388</v>
       </c>
       <c r="B346">
         <v>0.09</v>
@@ -3161,7 +3169,7 @@
     </row>
     <row r="347" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A347" s="1">
-        <v>44388</v>
+        <v>44389</v>
       </c>
       <c r="B347">
         <v>0.09</v>
@@ -3169,7 +3177,7 @@
     </row>
     <row r="348" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A348" s="1">
-        <v>44389</v>
+        <v>44390</v>
       </c>
       <c r="B348">
         <v>0.09</v>
@@ -3177,7 +3185,7 @@
     </row>
     <row r="349" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A349" s="1">
-        <v>44390</v>
+        <v>44391</v>
       </c>
       <c r="B349">
         <v>0.09</v>
@@ -3185,15 +3193,15 @@
     </row>
     <row r="350" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A350" s="1">
-        <v>44391</v>
+        <v>44392</v>
       </c>
       <c r="B350">
-        <v>0.09</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="351" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A351" s="1">
-        <v>44392</v>
+        <v>44393</v>
       </c>
       <c r="B351">
         <v>0.1</v>
@@ -3201,15 +3209,15 @@
     </row>
     <row r="352" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A352" s="1">
-        <v>44393</v>
+        <v>44394</v>
       </c>
       <c r="B352">
-        <v>0.1</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="353" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A353" s="1">
-        <v>44394</v>
+        <v>44395</v>
       </c>
       <c r="B353">
         <v>0.11</v>
@@ -3217,15 +3225,15 @@
     </row>
     <row r="354" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A354" s="1">
-        <v>44395</v>
+        <v>44396</v>
       </c>
       <c r="B354">
-        <v>0.11</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="355" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A355" s="1">
-        <v>44396</v>
+        <v>44397</v>
       </c>
       <c r="B355">
         <v>0.12</v>
@@ -3233,31 +3241,31 @@
     </row>
     <row r="356" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A356" s="1">
-        <v>44397</v>
+        <v>44398</v>
       </c>
       <c r="B356">
-        <v>0.12</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="357" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A357" s="1">
-        <v>44398</v>
+        <v>44399</v>
       </c>
       <c r="B357">
-        <v>0.13</v>
+        <v>0.14000000000000001</v>
       </c>
     </row>
     <row r="358" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A358" s="1">
-        <v>44399</v>
+        <v>44400</v>
       </c>
       <c r="B358">
-        <v>0.14000000000000001</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="359" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A359" s="1">
-        <v>44400</v>
+        <v>44401</v>
       </c>
       <c r="B359">
         <v>0.15</v>
@@ -3265,111 +3273,111 @@
     </row>
     <row r="360" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A360" s="1">
-        <v>44401</v>
+        <v>44402</v>
       </c>
       <c r="B360">
-        <v>0.15</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="361" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A361" s="1">
-        <v>44402</v>
+        <v>44403</v>
       </c>
       <c r="B361">
-        <v>0.16</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="362" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A362" s="1">
-        <v>44403</v>
+        <v>44404</v>
       </c>
       <c r="B362">
-        <v>0.17</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="363" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A363" s="1">
-        <v>44404</v>
+        <v>44405</v>
       </c>
       <c r="B363">
-        <v>0.18</v>
+        <v>0.19</v>
       </c>
     </row>
     <row r="364" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A364" s="1">
-        <v>44405</v>
+        <v>44406</v>
       </c>
       <c r="B364">
-        <v>0.19</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="365" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A365" s="1">
-        <v>44406</v>
+        <v>44407</v>
       </c>
       <c r="B365">
-        <v>0.2</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="366" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A366" s="1">
-        <v>44407</v>
+        <v>44408</v>
       </c>
       <c r="B366">
-        <v>0.21</v>
+        <v>0.23</v>
       </c>
     </row>
     <row r="367" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A367" s="1">
-        <v>44408</v>
+        <v>44409</v>
       </c>
       <c r="B367">
-        <v>0.23</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="368" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A368" s="1">
-        <v>44409</v>
+        <v>44410</v>
       </c>
       <c r="B368">
-        <v>0.24</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="369" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A369" s="1">
-        <v>44410</v>
+        <v>44411</v>
       </c>
       <c r="B369">
-        <v>0.25</v>
+        <v>0.26</v>
       </c>
     </row>
     <row r="370" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A370" s="1">
-        <v>44411</v>
+        <v>44412</v>
       </c>
       <c r="B370">
-        <v>0.26</v>
+        <v>0.27</v>
       </c>
     </row>
     <row r="371" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A371" s="1">
-        <v>44412</v>
+        <v>44413</v>
       </c>
       <c r="B371">
-        <v>0.27</v>
+        <v>0.28999999999999998</v>
       </c>
     </row>
     <row r="372" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A372" s="1">
-        <v>44413</v>
+        <v>44414</v>
       </c>
       <c r="B372">
-        <v>0.28999999999999998</v>
+        <v>0.31</v>
       </c>
     </row>
     <row r="373" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A373" s="1">
-        <v>44414</v>
+        <v>44415</v>
       </c>
       <c r="B373">
         <v>0.31</v>
@@ -3377,7 +3385,7 @@
     </row>
     <row r="374" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A374" s="1">
-        <v>44415</v>
+        <v>44416</v>
       </c>
       <c r="B374">
         <v>0.31</v>
@@ -3385,39 +3393,39 @@
     </row>
     <row r="375" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A375" s="1">
-        <v>44416</v>
+        <v>44417</v>
       </c>
       <c r="B375">
-        <v>0.31</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="376" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A376" s="1">
-        <v>44417</v>
+        <v>44418</v>
       </c>
       <c r="B376">
-        <v>0.33</v>
+        <v>0.34</v>
       </c>
     </row>
     <row r="377" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A377" s="1">
-        <v>44418</v>
+        <v>44419</v>
       </c>
       <c r="B377">
-        <v>0.34</v>
+        <v>0.36</v>
       </c>
     </row>
     <row r="378" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A378" s="1">
-        <v>44419</v>
+        <v>44420</v>
       </c>
       <c r="B378">
-        <v>0.36</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="379" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A379" s="1">
-        <v>44420</v>
+        <v>44421</v>
       </c>
       <c r="B379">
         <v>0.37</v>
@@ -3425,15 +3433,15 @@
     </row>
     <row r="380" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A380" s="1">
-        <v>44421</v>
+        <v>44422</v>
       </c>
       <c r="B380">
-        <v>0.37</v>
+        <v>0.38</v>
       </c>
     </row>
     <row r="381" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A381" s="1">
-        <v>44422</v>
+        <v>44423</v>
       </c>
       <c r="B381">
         <v>0.38</v>
@@ -3441,7 +3449,7 @@
     </row>
     <row r="382" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A382" s="1">
-        <v>44423</v>
+        <v>44424</v>
       </c>
       <c r="B382">
         <v>0.38</v>
@@ -3449,15 +3457,15 @@
     </row>
     <row r="383" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A383" s="1">
-        <v>44424</v>
+        <v>44425</v>
       </c>
       <c r="B383">
-        <v>0.38</v>
+        <v>0.39</v>
       </c>
     </row>
     <row r="384" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A384" s="1">
-        <v>44425</v>
+        <v>44426</v>
       </c>
       <c r="B384">
         <v>0.39</v>
@@ -3465,7 +3473,7 @@
     </row>
     <row r="385" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A385" s="1">
-        <v>44426</v>
+        <v>44427</v>
       </c>
       <c r="B385">
         <v>0.39</v>
@@ -3473,23 +3481,23 @@
     </row>
     <row r="386" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A386" s="1">
-        <v>44427</v>
+        <v>44428</v>
       </c>
       <c r="B386">
-        <v>0.39</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="387" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A387" s="1">
-        <v>44428</v>
+        <v>44429</v>
       </c>
       <c r="B387">
-        <v>0.4</v>
+        <v>0.42</v>
       </c>
     </row>
     <row r="388" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A388" s="1">
-        <v>44429</v>
+        <v>44430</v>
       </c>
       <c r="B388">
         <v>0.42</v>
@@ -3497,15 +3505,15 @@
     </row>
     <row r="389" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A389" s="1">
-        <v>44430</v>
+        <v>44431</v>
       </c>
       <c r="B389">
-        <v>0.42</v>
+        <v>0.43</v>
       </c>
     </row>
     <row r="390" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A390" s="1">
-        <v>44431</v>
+        <v>44432</v>
       </c>
       <c r="B390">
         <v>0.43</v>
@@ -3513,31 +3521,31 @@
     </row>
     <row r="391" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A391" s="1">
-        <v>44432</v>
+        <v>44433</v>
       </c>
       <c r="B391">
-        <v>0.43</v>
+        <v>0.44</v>
       </c>
     </row>
     <row r="392" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A392" s="1">
-        <v>44433</v>
+        <v>44434</v>
       </c>
       <c r="B392">
-        <v>0.44</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="393" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A393" s="1">
-        <v>44434</v>
+        <v>44435</v>
       </c>
       <c r="B393">
-        <v>0.45</v>
+        <v>0.46</v>
       </c>
     </row>
     <row r="394" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A394" s="1">
-        <v>44435</v>
+        <v>44436</v>
       </c>
       <c r="B394">
         <v>0.46</v>
@@ -3545,23 +3553,23 @@
     </row>
     <row r="395" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A395" s="1">
-        <v>44436</v>
+        <v>44437</v>
       </c>
       <c r="B395">
-        <v>0.46</v>
+        <v>0.47</v>
       </c>
     </row>
     <row r="396" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A396" s="1">
-        <v>44437</v>
+        <v>44438</v>
       </c>
       <c r="B396">
-        <v>0.47</v>
+        <v>0.48</v>
       </c>
     </row>
     <row r="397" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A397" s="1">
-        <v>44438</v>
+        <v>44439</v>
       </c>
       <c r="B397">
         <v>0.48</v>
@@ -3569,15 +3577,15 @@
     </row>
     <row r="398" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A398" s="1">
-        <v>44439</v>
+        <v>44440</v>
       </c>
       <c r="B398">
-        <v>0.48</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="399" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A399" s="1">
-        <v>44440</v>
+        <v>44441</v>
       </c>
       <c r="B399">
         <v>0.5</v>
@@ -3585,7 +3593,7 @@
     </row>
     <row r="400" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A400" s="1">
-        <v>44441</v>
+        <v>44442</v>
       </c>
       <c r="B400">
         <v>0.5</v>
@@ -3593,23 +3601,23 @@
     </row>
     <row r="401" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A401" s="1">
-        <v>44442</v>
+        <v>44443</v>
       </c>
       <c r="B401">
-        <v>0.5</v>
+        <v>0.51</v>
       </c>
     </row>
     <row r="402" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A402" s="1">
-        <v>44443</v>
+        <v>44444</v>
       </c>
       <c r="B402">
-        <v>0.51</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="403" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A403" s="1">
-        <v>44444</v>
+        <v>44445</v>
       </c>
       <c r="B403">
         <v>0.5</v>
@@ -3617,7 +3625,7 @@
     </row>
     <row r="404" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A404" s="1">
-        <v>44445</v>
+        <v>44446</v>
       </c>
       <c r="B404">
         <v>0.5</v>
@@ -3625,23 +3633,23 @@
     </row>
     <row r="405" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A405" s="1">
-        <v>44446</v>
+        <v>44447</v>
       </c>
       <c r="B405">
-        <v>0.5</v>
+        <v>0.49</v>
       </c>
     </row>
     <row r="406" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A406" s="1">
-        <v>44447</v>
+        <v>44448</v>
       </c>
       <c r="B406">
-        <v>0.49</v>
+        <v>0.48</v>
       </c>
     </row>
     <row r="407" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A407" s="1">
-        <v>44448</v>
+        <v>44449</v>
       </c>
       <c r="B407">
         <v>0.48</v>
@@ -3649,15 +3657,15 @@
     </row>
     <row r="408" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A408" s="1">
-        <v>44449</v>
+        <v>44450</v>
       </c>
       <c r="B408">
-        <v>0.48</v>
+        <v>0.47</v>
       </c>
     </row>
     <row r="409" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A409" s="1">
-        <v>44450</v>
+        <v>44451</v>
       </c>
       <c r="B409">
         <v>0.47</v>
@@ -3665,7 +3673,7 @@
     </row>
     <row r="410" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A410" s="1">
-        <v>44451</v>
+        <v>44452</v>
       </c>
       <c r="B410">
         <v>0.47</v>
@@ -3673,23 +3681,23 @@
     </row>
     <row r="411" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A411" s="1">
-        <v>44452</v>
+        <v>44453</v>
       </c>
       <c r="B411">
-        <v>0.47</v>
+        <v>0.48</v>
       </c>
     </row>
     <row r="412" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A412" s="1">
-        <v>44453</v>
+        <v>44454</v>
       </c>
       <c r="B412">
-        <v>0.48</v>
+        <v>0.47</v>
       </c>
     </row>
     <row r="413" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A413" s="1">
-        <v>44454</v>
+        <v>44455</v>
       </c>
       <c r="B413">
         <v>0.47</v>
@@ -3697,15 +3705,15 @@
     </row>
     <row r="414" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A414" s="1">
-        <v>44455</v>
+        <v>44456</v>
       </c>
       <c r="B414">
-        <v>0.47</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="415" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A415" s="1">
-        <v>44456</v>
+        <v>44457</v>
       </c>
       <c r="B415">
         <v>0.45</v>
@@ -3713,47 +3721,47 @@
     </row>
     <row r="416" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A416" s="1">
-        <v>44457</v>
+        <v>44458</v>
       </c>
       <c r="B416">
-        <v>0.45</v>
+        <v>0.44</v>
       </c>
     </row>
     <row r="417" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A417" s="1">
-        <v>44458</v>
+        <v>44459</v>
       </c>
       <c r="B417">
-        <v>0.44</v>
+        <v>0.43</v>
       </c>
     </row>
     <row r="418" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A418" s="1">
-        <v>44459</v>
+        <v>44460</v>
       </c>
       <c r="B418">
-        <v>0.43</v>
+        <v>0.41</v>
       </c>
     </row>
     <row r="419" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A419" s="1">
-        <v>44460</v>
+        <v>44461</v>
       </c>
       <c r="B419">
-        <v>0.41</v>
+        <v>0.39</v>
       </c>
     </row>
     <row r="420" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A420" s="1">
-        <v>44461</v>
+        <v>44462</v>
       </c>
       <c r="B420">
-        <v>0.39</v>
+        <v>0.38</v>
       </c>
     </row>
     <row r="421" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A421" s="1">
-        <v>44462</v>
+        <v>44463</v>
       </c>
       <c r="B421">
         <v>0.38</v>
@@ -3761,31 +3769,31 @@
     </row>
     <row r="422" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A422" s="1">
-        <v>44463</v>
+        <v>44464</v>
       </c>
       <c r="B422">
-        <v>0.38</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="423" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A423" s="1">
-        <v>44464</v>
+        <v>44465</v>
       </c>
       <c r="B423">
-        <v>0.37</v>
+        <v>0.36</v>
       </c>
     </row>
     <row r="424" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A424" s="1">
-        <v>44465</v>
+        <v>44466</v>
       </c>
       <c r="B424">
-        <v>0.36</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="425" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A425" s="1">
-        <v>44466</v>
+        <v>44467</v>
       </c>
       <c r="B425">
         <v>0.35</v>
@@ -3793,17 +3801,9 @@
     </row>
     <row r="426" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A426" s="1">
-        <v>44467</v>
+        <v>44468</v>
       </c>
       <c r="B426">
-        <v>0.35</v>
-      </c>
-    </row>
-    <row r="427" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A427" s="1">
-        <v>44468</v>
-      </c>
-      <c r="B427">
         <v>0.34</v>
       </c>
     </row>

</xml_diff>